<commit_message>
Bloom Cnt UI에 표시
</commit_message>
<xml_diff>
--- a/Assets/Resources/Jsons/NormalQuest.xlsx
+++ b/Assets/Resources/Jsons/NormalQuest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56d3f5b802244a48/바탕 화면/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56d3f5b802244a48/문서/GitHub/Blossom-Company/Assets/Resources/Jsons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17D63BBB-0FDA-4700-8AC0-09AD1406FDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{17D63BBB-0FDA-4700-8AC0-09AD1406FDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7353E3AD-ADE1-4B8E-8EFD-DF9B55289F27}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BF3C0F20-860A-4F39-963E-B037A06D84F0}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" xr2:uid="{BF3C0F20-860A-4F39-963E-B037A06D84F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,6 +116,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -418,7 +422,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -442,27 +446,27 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>